<commit_message>
Add Readme and pdf files
</commit_message>
<xml_diff>
--- a/ZJUNlict_Communication_Protocol_V1.6.xlsx
+++ b/ZJUNlict_Communication_Protocol_V1.6.xlsx
@@ -88,10 +88,10 @@
     <t>Example:</t>
   </si>
   <si>
-    <t>4F 12 34 30 08 00 02 40 00 08 02 60 00 08 00 50 00 08 00 00 00 00 00 00 32 32 32</t>
-  </si>
-  <si>
-    <t>4F 12 34 30 58 00 02 40 00 08 02 60 00 08 00 50 00 08 00 00 00 00 00 00 32 32 32</t>
+    <t>4F 12 34 30 08 00 02 40 00 08 02 60 00 08 00 50 00 08 00 00 00 00 32 32 32</t>
+  </si>
+  <si>
+    <t>4F 12 34 30 58 00 02 40 00 08 02 60 00 08 00 50 00 08 00 00 00 00 32 32 32</t>
   </si>
   <si>
     <t>Robot4 Config</t>
@@ -310,7 +310,7 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>0xF0</t>
+    <t>Package_Header</t>
   </si>
   <si>
     <t>Frequency_For_TX(RF_CH)</t>
@@ -417,8 +417,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -464,27 +464,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -496,29 +475,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -547,21 +503,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -578,8 +519,74 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,14 +601,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -640,19 +640,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,37 +706,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,6 +748,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -730,97 +820,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,6 +1331,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1365,13 +1374,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1394,41 +1407,28 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1446,130 +1446,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2112,7 +2112,7 @@
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2136,7 +2136,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="2" ht="15.75"/>
+    <row r="3" ht="15.75" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2174,7 +2175,7 @@
       </c>
       <c r="N3" s="57"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" ht="15.75" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2237,7 @@
       <c r="K5" s="35"/>
       <c r="N5" s="35"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" ht="15.75" spans="1:14">
       <c r="A6" s="15"/>
       <c r="B6" s="16">
         <v>2</v>
@@ -2258,7 +2259,7 @@
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" ht="15.75" spans="1:14">
       <c r="A7" s="15"/>
       <c r="B7" s="16">
         <v>3</v>
@@ -2448,7 +2449,7 @@
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" ht="15.75" spans="1:14">
+    <row r="15" spans="1:14">
       <c r="A15" s="15"/>
       <c r="B15" s="16">
         <v>11</v>
@@ -2472,7 +2473,7 @@
       <c r="M15" s="35"/>
       <c r="N15" s="35"/>
     </row>
-    <row r="16" ht="15.75" spans="1:14">
+    <row r="16" spans="1:14">
       <c r="A16" s="15"/>
       <c r="B16" s="20">
         <v>12</v>
@@ -2626,7 +2627,7 @@
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" ht="15.75" spans="1:14">
       <c r="A22" s="15"/>
       <c r="B22" s="16">
         <v>18</v>
@@ -2660,7 +2661,7 @@
       <c r="M22" s="35"/>
       <c r="N22" s="35"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" ht="15.75" spans="1:14">
       <c r="A23" s="15"/>
       <c r="B23" s="16">
         <v>19</v>
@@ -2694,7 +2695,7 @@
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" ht="15.75" spans="1:14">
       <c r="A24" s="15"/>
       <c r="B24" s="30">
         <v>20</v>
@@ -2728,7 +2729,7 @@
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" ht="16.5" spans="1:14">
       <c r="A25" s="10" t="s">
         <v>61</v>
       </c>
@@ -2766,7 +2767,7 @@
       <c r="M25" s="35"/>
       <c r="N25" s="35"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" ht="15.75" spans="1:14">
       <c r="A26" s="15"/>
       <c r="B26" s="26">
         <v>22</v>
@@ -2800,7 +2801,7 @@
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" ht="15.75" spans="1:14">
       <c r="A27" s="15"/>
       <c r="B27" s="26">
         <v>23</v>
@@ -2834,7 +2835,7 @@
       <c r="M27" s="35"/>
       <c r="N27" s="35"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" ht="15.75" spans="1:14">
       <c r="A28" s="15"/>
       <c r="B28" s="27">
         <v>24</v>
@@ -2886,7 +2887,7 @@
       <c r="M29" s="35"/>
       <c r="N29" s="35"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" ht="15.75" spans="1:14">
       <c r="A32" s="36" t="s">
         <v>96</v>
       </c>
@@ -2904,7 +2905,7 @@
       <c r="M32" s="35"/>
       <c r="N32" s="35"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" ht="15.75" spans="1:14">
       <c r="A33" s="37" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +2979,7 @@
       <c r="M34" s="35"/>
       <c r="N34" s="35"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" ht="15.75" spans="1:14">
       <c r="A35" s="41" t="s">
         <v>99</v>
       </c>
@@ -3016,7 +3017,7 @@
       <c r="M35" s="66"/>
       <c r="N35" s="67"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" ht="15.75" spans="1:12">
       <c r="A36" s="41" t="s">
         <v>101</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" ht="15.75" spans="1:14">
       <c r="A37" s="41" t="s">
         <v>102</v>
       </c>
@@ -3092,7 +3093,7 @@
       </c>
       <c r="N37" s="65"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" ht="15.75" spans="1:14">
       <c r="A38" s="41" t="s">
         <v>105</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" ht="15.75" spans="1:14">
       <c r="A39" s="41" t="s">
         <v>109</v>
       </c>
@@ -3199,7 +3200,7 @@
       <c r="M42" s="35"/>
       <c r="N42" s="35"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" ht="15.75" spans="1:14">
       <c r="A43" s="36" t="s">
         <v>111</v>
       </c>
@@ -3217,7 +3218,7 @@
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" ht="15.75" spans="1:14">
       <c r="A44" s="37" t="s">
         <v>1</v>
       </c>
@@ -3250,7 +3251,7 @@
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" ht="15.75" spans="1:11">
       <c r="A45" s="39" t="s">
         <v>4</v>
       </c>
@@ -3269,7 +3270,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="35"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" ht="15.75" spans="1:14">
       <c r="A46" s="41" t="s">
         <v>113</v>
       </c>
@@ -3290,7 +3291,7 @@
       <c r="M46" s="35"/>
       <c r="N46" s="35"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" ht="15.75" spans="1:14">
       <c r="A47" s="41" t="s">
         <v>115</v>
       </c>
@@ -3341,7 +3342,7 @@
       <c r="M48" s="35"/>
       <c r="N48" s="35"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" ht="15.75" spans="1:14">
       <c r="A49" s="41" t="s">
         <v>121</v>
       </c>
@@ -3361,7 +3362,7 @@
       <c r="M49" s="35"/>
       <c r="N49" s="35"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" ht="15.75" spans="1:10">
       <c r="A50" s="41" t="s">
         <v>122</v>
       </c>
@@ -3397,7 +3398,7 @@
       <c r="M51" s="35"/>
       <c r="N51" s="35"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" ht="15.75" spans="1:14">
       <c r="A52" s="39"/>
       <c r="B52" s="42">
         <v>7</v>
@@ -3435,7 +3436,7 @@
       <c r="M53" s="35"/>
       <c r="N53" s="35"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" ht="15.75" spans="1:14">
       <c r="A54" s="39"/>
       <c r="B54" s="42">
         <v>9</v>
@@ -3468,7 +3469,7 @@
       <c r="I55" s="54"/>
       <c r="J55" s="70"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" ht="15.75" spans="1:10">
       <c r="A56" s="39"/>
       <c r="B56" s="42">
         <v>11</v>
@@ -3498,7 +3499,7 @@
       <c r="I57" s="54"/>
       <c r="J57" s="70"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" ht="15.75" spans="1:10">
       <c r="A58" s="39"/>
       <c r="B58" s="42">
         <v>13</v>
@@ -3528,7 +3529,7 @@
       <c r="I59" s="54"/>
       <c r="J59" s="70"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" ht="15.75" spans="1:10">
       <c r="A60" s="39"/>
       <c r="B60" s="42">
         <v>15</v>
@@ -3558,7 +3559,7 @@
       <c r="I61" s="54"/>
       <c r="J61" s="70"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" ht="15.75" spans="1:10">
       <c r="A62" s="39"/>
       <c r="B62" s="42">
         <v>17</v>
@@ -3588,7 +3589,7 @@
       <c r="I63" s="54"/>
       <c r="J63" s="70"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" ht="15.75" spans="1:10">
       <c r="A64" s="39"/>
       <c r="B64" s="42">
         <v>19</v>
@@ -3618,7 +3619,7 @@
       <c r="I65" s="54"/>
       <c r="J65" s="70"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" ht="15.75" spans="1:10">
       <c r="A66" s="39"/>
       <c r="B66" s="42">
         <v>21</v>
@@ -3648,7 +3649,7 @@
       <c r="I67" s="54"/>
       <c r="J67" s="70"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" ht="15.75" spans="1:10">
       <c r="A68" s="39"/>
       <c r="B68" s="42">
         <v>23</v>
@@ -3676,7 +3677,7 @@
       <c r="I69" s="54"/>
       <c r="J69" s="70"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" ht="15.75" spans="1:10">
       <c r="A70" s="39"/>
       <c r="B70" s="42">
         <v>25</v>

</xml_diff>